<commit_message>
FIX: Several fixes on the FV function
(1+x)^(1+y) was stringifyfied incorrectly
We still need work on this

FV now returns currency

FV(-1,-2,1) should return #DIV/0! not #NUM!
</commit_message>
<xml_diff>
--- a/xlsx/tests/calc_tests/FV.xlsx
+++ b/xlsx/tests/calc_tests/FV.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nhatcher/IronCalc/IronCalc/xlsx/tests/calc_tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332C447B-24F6-DD4D-AAFB-09AFF14A1CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82202378-E09B-B147-97C2-782728929E70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" xr2:uid="{DE9EEB5E-A344-114F-A3A7-2DF82E6E63E7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" activeTab="1" xr2:uid="{DE9EEB5E-A344-114F-A3A7-2DF82E6E63E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -153,9 +154,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -193,7 +194,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -299,7 +300,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -441,7 +442,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -451,7 +452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74040971-AB19-524D-827E-880EEF58350E}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1025,4 +1026,29 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{891220E0-5814-A249-9EBB-0E08390C4872}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="e">
+        <f>FV(-1,-2,1)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="B1" s="3" t="e">
+        <f>FV(-3, -3.5, 1)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>